<commit_message>
combined native and scanned pdf processing + excel writing
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x\Documents\GitHub\Proiect-RPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C2E66A-54E7-4B69-BC29-434CBD7EFB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC4B26F-B10E-4498-8536-FDADC6CAA36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{19CE312D-A43A-4F9E-8351-09B765A54963}"/>
+    <workbookView xWindow="4800" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{3737AAAE-4B33-4EE7-8C33-9D8A05A71FF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,8 +390,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D269F5-1A61-486A-BC89-F7636B137136}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DC0D05-5607-473D-ABCF-8195F41B21A4}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,17 +415,25 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>1122334455667</v>
+        <v>6001016330261</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1122334455667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>9876543210011</v>
       </c>
     </row>

</xml_diff>